<commit_message>
Not messing with it rn
Separate script for I/O is too difficult right now. Moving on
</commit_message>
<xml_diff>
--- a/Outputs/bankrolls.xlsx
+++ b/Outputs/bankrolls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.phillips\Documents\GitHub\Poker-Stats\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E485FB-CEC7-4053-A09E-1503EB349586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728245D7-D5BA-4932-B7F6-B2C03F92A4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -582,37 +582,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1804,444 +1773,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-DBD4-4F74-B56F-8A55AB727B5A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="713638751"/>
-        <c:axId val="715084319"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="713638751"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="715084319"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="715084319"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-            <a:prstDash val="solid"/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="713638751"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Cheyenne </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Bankroll</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Bankrolls!$A$2:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>4 09</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4 16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4 19</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4 24</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4 26</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4 29</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5 04</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5 13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5 17</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5 20</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5 24</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5 27</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5 28</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5 31</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Bankrolls!$X$2:$X$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0D11-4B3E-9E67-28E10233EE3C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Bankrolls!$A$2:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>4 09</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4 16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4 19</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4 24</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4 26</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4 29</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5 04</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5 13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5 17</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5 20</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5 24</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5 27</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5 28</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5 31</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Bankrolls!$Y$2:$Y$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35.200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35.200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45.2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45.2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>65.2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>65.2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>65.2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>65.2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0D11-4B3E-9E67-28E10233EE3C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2518,42 +2049,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2861,8 +2356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V21" sqref="V21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Relative WASD added to a bunch of things
</commit_message>
<xml_diff>
--- a/Outputs/bankrolls.xlsx
+++ b/Outputs/bankrolls.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\OneDrive\Documents\GitHub\Poker-Stats\Outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.phillips\Documents\GitHub\Poker-Stats\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4847A235-BBD5-4A50-A4C0-0F756C4C21D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C05B85-5492-4FCC-96AF-663256144FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1655,15 +1655,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1990,8 +1990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Preparing to debug 3-betting
</commit_message>
<xml_diff>
--- a/Outputs/bankrolls.xlsx
+++ b/Outputs/bankrolls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.phillips\Documents\GitHub\Poker-Stats\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C05B85-5492-4FCC-96AF-663256144FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F2A675-17AE-4C78-8CDC-2086CFB50305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>06/17/21</t>
+  </si>
+  <si>
+    <t>06/21/21</t>
   </si>
 </sst>
 </file>
@@ -246,9 +249,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Bankrolls!$A$2:$A$20</c:f>
+              <c:f>Bankrolls!$A$2:$A$21</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>04/09/21</c:v>
                 </c:pt>
@@ -305,16 +308,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>06/17/21</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>06/21/21</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Bankrolls!$C$2:$C$20</c:f>
+              <c:f>Bankrolls!$C$2:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>-15.44</c:v>
                 </c:pt>
@@ -371,6 +377,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>202.13</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>216.44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -378,7 +387,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1DC6-4D2E-80C6-754EDFDB9A38}"/>
+              <c16:uniqueId val="{00000000-230C-479F-8014-97E4E98B9323}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -590,9 +599,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Bankrolls!$A$2:$A$20</c:f>
+              <c:f>Bankrolls!$A$2:$A$21</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>04/09/21</c:v>
                 </c:pt>
@@ -649,16 +658,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>06/17/21</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>06/21/21</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Bankrolls!$H$2:$H$20</c:f>
+              <c:f>Bankrolls!$H$2:$H$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -715,6 +727,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>-130.18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-123.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -722,7 +737,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9CBD-442A-B637-8C31B74B5F84}"/>
+              <c16:uniqueId val="{00000000-EBA6-4614-A73B-E13B87F69B18}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -933,9 +948,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Bankrolls!$A$2:$A$20</c:f>
+              <c:f>Bankrolls!$A$2:$A$21</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>04/09/21</c:v>
                 </c:pt>
@@ -992,16 +1007,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>06/17/21</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>06/21/21</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Bankrolls!$M$2:$M$20</c:f>
+              <c:f>Bankrolls!$M$2:$M$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>41.56</c:v>
                 </c:pt>
@@ -1058,6 +1076,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>483.29</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>461.32000000000011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1065,7 +1086,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-98AE-4B5D-8B41-06B75DDA382A}"/>
+              <c16:uniqueId val="{00000000-C993-474D-BE84-C352622B8B28}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1276,9 +1297,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Bankrolls!$A$2:$A$20</c:f>
+              <c:f>Bankrolls!$A$2:$A$21</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>04/09/21</c:v>
                 </c:pt>
@@ -1335,16 +1356,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>06/17/21</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>06/21/21</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Bankrolls!$R$2:$R$20</c:f>
+              <c:f>Bankrolls!$R$2:$R$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>-26.12</c:v>
                 </c:pt>
@@ -1401,6 +1425,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>-41.859999999999971</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-40.979999999999968</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1408,7 +1435,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C62E-4936-99D0-D32F10039C7A}"/>
+              <c16:uniqueId val="{00000000-143F-4EDC-A86D-A15D08827DF4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1988,10 +2015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2868,6 +2895,47 @@
         <v>107.23</v>
       </c>
     </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21">
+        <v>216.44</v>
+      </c>
+      <c r="D21">
+        <v>277.77</v>
+      </c>
+      <c r="E21">
+        <v>61.330000000000013</v>
+      </c>
+      <c r="H21">
+        <v>-123.4</v>
+      </c>
+      <c r="I21">
+        <v>35.630000000000003</v>
+      </c>
+      <c r="J21">
+        <v>159.03</v>
+      </c>
+      <c r="M21">
+        <v>461.32000000000011</v>
+      </c>
+      <c r="N21">
+        <v>471.36999999999989</v>
+      </c>
+      <c r="O21">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="R21">
+        <v>-40.979999999999968</v>
+      </c>
+      <c r="S21">
+        <v>66.25</v>
+      </c>
+      <c r="T21">
+        <v>107.23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
main loop changed from while to for
Avoid future infinite loops
</commit_message>
<xml_diff>
--- a/Outputs/bankrolls.xlsx
+++ b/Outputs/bankrolls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.phillips\Documents\GitHub\Poker-Stats\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F2A675-17AE-4C78-8CDC-2086CFB50305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E633FEA-940F-4A02-8F05-F05E536C9CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1684,13 +1684,13 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2018,7 +2018,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>